<commit_message>
add GenDbChangeLogCommand and UpdateDbChangeLogCommand.
</commit_message>
<xml_diff>
--- a/src/test/resources/xlsxFiles/genlog.xlsx
+++ b/src/test/resources/xlsxFiles/genlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xihu_\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projs\auto-test\src\test\resources\xlsxFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD6AE8E-51D4-4593-B4DE-3D36DEEF3DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66791F6-FFDC-499F-93D9-584CB68EAE05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,89 +38,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>genDbChangeLog</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>users</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t>{"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>"file","target":"C:\\projs\\auto-test\\src\\test\\resources\\exportDb\\db.conf","path":"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>work/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>download/gen1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>xml</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Meiryo UI"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>"}</t>
-    </r>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -248,6 +166,88 @@
       </rPr>
       <t>"
 }</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>generateChangeLog</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>{"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>"file","target":"C:\\projs\\auto-test\\src\\test\\resources\\exportDb\\db.conf","path":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>work/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>download/gen1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>xml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>","genType":"data"}</t>
     </r>
     <phoneticPr fontId="1"/>
   </si>
@@ -757,10 +757,10 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="8.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
@@ -768,7 +768,7 @@
     <col min="4" max="4" width="56.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="16.5">
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
@@ -779,44 +779,44 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="14.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="147">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="16.5">
       <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>